<commit_message>
renames parameters.sigma -> prob.sigma constants -> parameters sitchers -> events_active input_cons -> parameters_upd
</commit_message>
<xml_diff>
--- a/cases/story_2/conditions.xlsx
+++ b/cases/story_2/conditions.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Julia\dev\HetaSimulator\cases\story_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\HetaSimulator.jl\cases\story_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30933698-427B-4FDD-B206-FD449A4281F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7480" windowHeight="2460"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="conditions" sheetId="1" r:id="rId1"/>
@@ -24,15 +25,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>constants.k1</t>
-  </si>
-  <si>
-    <t>constants.k2</t>
-  </si>
-  <si>
-    <t>constants.k3</t>
-  </si>
-  <si>
     <t>saveat[]</t>
   </si>
   <si>
@@ -58,12 +50,21 @@
   </si>
   <si>
     <t>b;c</t>
+  </si>
+  <si>
+    <t>parameters.k1</t>
+  </si>
+  <si>
+    <t>parameters.k2</t>
+  </si>
+  <si>
+    <t>parameters.k3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -546,48 +547,48 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="20% — акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% — акцент2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% — акцент3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% — акцент4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% — акцент5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% — акцент6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% — акцент1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% — акцент2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% — акцент3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% — акцент4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% — акцент5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% — акцент6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% — акцент1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% — акцент2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% — акцент3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% — акцент4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% — акцент5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% — акцент6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Акцент1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Акцент2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Акцент3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Акцент4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Акцент5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Акцент6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Ввод " xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Вывод" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Вычисление" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Заголовок 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Заголовок 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Заголовок 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Заголовок 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Итог" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Контрольная ячейка" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Название" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Нейтральный" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Плохой" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Пояснение" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Примечание" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Связанная ячейка" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Текст предупреждения" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Хороший" xfId="6" builtinId="26" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -864,39 +865,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="22.88671875" customWidth="1"/>
+    <col min="3" max="3" width="25.21875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>7</v>
       </c>
       <c r="C2">
         <v>1E-3</v>
@@ -905,26 +912,26 @@
         <v>0.02</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F2">
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>1E-3</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1">
         <v>1E-3</v>
@@ -936,9 +943,9 @@
         <v>250</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1">
         <v>1E-4</v>
@@ -950,7 +957,7 @@
         <v>1000</v>
       </c>
       <c r="G5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>